<commit_message>
Revert "committed by ram.sin"
This reverts commit 76ecf8dae882a60a4bca56c4c3fd27d7cc6e5bcf.
</commit_message>
<xml_diff>
--- a/src/main/java/lomt/pearson/fileupload/english/gse/ingestion/Gse_Ingestion_Template.xlsx
+++ b/src/main/java/lomt/pearson/fileupload/english/gse/ingestion/Gse_Ingestion_Template.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\lomt_automation\src\main\java\lomt\pearson\fileupload\english\gse\ingestion\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" tabRatio="442" activeTab="1"/>
   </bookViews>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="134">
   <si>
     <t>To be populated - ignored by the import</t>
   </si>
@@ -422,31 +417,13 @@
   </si>
   <si>
     <t>GLSI16099C0</t>
-  </si>
-  <si>
-    <t>GLSI7676A0</t>
-  </si>
-  <si>
-    <t>Can respond to ideas and suggestions in informal discussions on  January</t>
-  </si>
-  <si>
-    <t>GLGR3232</t>
-  </si>
-  <si>
-    <t>GLVC3232c</t>
-  </si>
-  <si>
-    <t>Can use language related to adverts and brands on January</t>
-  </si>
-  <si>
-    <t>Can link clauses and sentences with a range of basic connectors  on January.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -494,25 +471,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -542,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -585,15 +550,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -655,7 +611,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -690,7 +646,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -867,29 +823,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="26" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="1"/>
     </row>
   </sheetData>
@@ -898,14 +854,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AA23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="6"/>
     <col min="2" max="2" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
@@ -932,7 +888,7 @@
     <col min="26" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="27" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1013,10 +969,10 @@
       </c>
       <c r="AA1" s="3"/>
     </row>
-    <row r="2" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="27" customHeight="1">
       <c r="A2" s="8"/>
-      <c r="B2" s="13" t="s">
-        <v>134</v>
+      <c r="B2" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>26</v>
@@ -1032,7 +988,7 @@
         <v>29</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>135</v>
+        <v>94</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>30</v>
@@ -1072,18 +1028,20 @@
       </c>
       <c r="AA2" s="3"/>
     </row>
-    <row r="3" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="27" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="14" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="F3" s="8" t="s">
         <v>28</v>
       </c>
@@ -1091,59 +1049,47 @@
         <v>29</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="J3" s="8">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>104</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="9"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
-      <c r="U3" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="U3" s="8"/>
       <c r="V3" s="8"/>
       <c r="W3" s="8" t="s">
         <v>106</v>
       </c>
       <c r="X3" s="8"/>
       <c r="Y3" s="8"/>
-      <c r="Z3" s="8" t="s">
-        <v>34</v>
-      </c>
+      <c r="Z3" s="8"/>
       <c r="AA3" s="3"/>
     </row>
-    <row r="4" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="27" customHeight="1">
       <c r="A4" s="8"/>
       <c r="B4" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>35</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="C4" s="8"/>
       <c r="D4" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>28</v>
@@ -1152,20 +1098,26 @@
         <v>29</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J4" s="8">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="9"/>
+        <v>43</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>90</v>
+      </c>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
@@ -1177,23 +1129,25 @@
       <c r="W4" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
+      <c r="X4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y4" s="8" t="s">
+        <v>40</v>
+      </c>
       <c r="Z4" s="8"/>
       <c r="AA4" s="3"/>
     </row>
-    <row r="5" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="27" customHeight="1">
       <c r="A5" s="8"/>
       <c r="B5" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="E5" s="8"/>
       <c r="F5" s="8" t="s">
         <v>28</v>
       </c>
@@ -1201,25 +1155,25 @@
         <v>29</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J5" s="8">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>90</v>
+        <v>47</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
@@ -1227,30 +1181,36 @@
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
-      <c r="U5" s="8"/>
+      <c r="U5" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="V5" s="8"/>
       <c r="W5" s="8" t="s">
-        <v>106</v>
+        <v>49</v>
       </c>
       <c r="X5" s="8" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="Y5" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z5" s="8"/>
       <c r="AA5" s="3"/>
     </row>
-    <row r="6" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="27" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="8"/>
+        <v>82</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="D6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="F6" s="8" t="s">
         <v>28</v>
       </c>
@@ -1258,25 +1218,25 @@
         <v>29</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J6" s="8">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
@@ -1284,36 +1244,30 @@
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
-      <c r="U6" s="8" t="s">
-        <v>48</v>
-      </c>
+      <c r="U6" s="8"/>
       <c r="V6" s="8"/>
       <c r="W6" s="8" t="s">
-        <v>49</v>
+        <v>106</v>
       </c>
       <c r="X6" s="8" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="Y6" s="8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="Z6" s="8"/>
       <c r="AA6" s="3"/>
     </row>
-    <row r="7" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="27" customHeight="1">
       <c r="A7" s="8"/>
       <c r="B7" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>51</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="C7" s="8"/>
       <c r="D7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="E7" s="8"/>
       <c r="F7" s="8" t="s">
         <v>28</v>
       </c>
@@ -1321,25 +1275,25 @@
         <v>29</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J7" s="8">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>120</v>
+        <v>60</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
@@ -1347,30 +1301,34 @@
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
-      <c r="U7" s="8"/>
+      <c r="U7" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="V7" s="8"/>
-      <c r="W7" s="8" t="s">
-        <v>106</v>
-      </c>
+      <c r="W7" s="8"/>
       <c r="X7" s="8" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="Y7" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Z7" s="8"/>
       <c r="AA7" s="3"/>
     </row>
-    <row r="8" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="27" customHeight="1">
       <c r="A8" s="8"/>
       <c r="B8" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="8"/>
+        <v>84</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="D8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="8"/>
+      <c r="E8" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="F8" s="8" t="s">
         <v>28</v>
       </c>
@@ -1378,25 +1336,25 @@
         <v>29</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J8" s="8">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="N8" s="7" t="s">
-        <v>91</v>
+        <v>63</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
@@ -1404,28 +1362,24 @@
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
-      <c r="U8" s="8" t="s">
-        <v>61</v>
-      </c>
+      <c r="U8" s="8"/>
       <c r="V8" s="8"/>
       <c r="W8" s="8"/>
       <c r="X8" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="Y8" s="8" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="Z8" s="8"/>
       <c r="AA8" s="3"/>
     </row>
-    <row r="9" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="27" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>62</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C9" s="8"/>
       <c r="D9" s="8" t="s">
         <v>27</v>
       </c>
@@ -1433,32 +1387,30 @@
         <v>42</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J9" s="8">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>92</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
@@ -1467,20 +1419,22 @@
       <c r="T9" s="4"/>
       <c r="U9" s="8"/>
       <c r="V9" s="8"/>
-      <c r="W9" s="8"/>
+      <c r="W9" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="X9" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="Y9" s="8" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="Z9" s="8"/>
       <c r="AA9" s="3"/>
     </row>
-    <row r="10" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="27" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="14" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8" t="s">
@@ -1493,26 +1447,22 @@
         <v>57</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J10" s="8">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="K10" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="L10" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>66</v>
-      </c>
+      <c r="L10" s="8"/>
+      <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
@@ -1523,7 +1473,7 @@
       <c r="U10" s="8"/>
       <c r="V10" s="8"/>
       <c r="W10" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="X10" s="8" t="s">
         <v>50</v>
@@ -1531,13 +1481,15 @@
       <c r="Y10" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="Z10" s="8"/>
+      <c r="Z10" s="8" t="s">
+        <v>69</v>
+      </c>
       <c r="AA10" s="3"/>
     </row>
-    <row r="11" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" ht="27" customHeight="1">
       <c r="A11" s="8"/>
       <c r="B11" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8" t="s">
@@ -1547,22 +1499,22 @@
         <v>42</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J11" s="8">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="L11" s="8"/>
       <c r="M11" s="4"/>
@@ -1576,23 +1528,23 @@
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
       <c r="W11" s="8" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="X11" s="8" t="s">
         <v>50</v>
       </c>
       <c r="Y11" s="8" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="Z11" s="8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="AA11" s="3"/>
     </row>
-    <row r="12" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" ht="27" customHeight="1">
       <c r="A12" s="8"/>
       <c r="B12" s="14" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8" t="s">
@@ -1644,293 +1596,299 @@
       </c>
       <c r="AA12" s="3"/>
     </row>
-    <row r="13" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" s="11" customFormat="1" ht="27" customHeight="1">
       <c r="A13" s="8"/>
-      <c r="B13" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C13" s="8"/>
+      <c r="B13" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="8">
+        <v>79566</v>
+      </c>
       <c r="D13" s="8" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>42</v>
+        <v>109</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>28</v>
+        <v>110</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J13" s="8">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L13" s="8"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="R13" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="S13" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="T13" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="U13" s="8" t="s">
+        <v>116</v>
+      </c>
       <c r="V13" s="8"/>
-      <c r="W13" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="X13" s="8" t="s">
-        <v>50</v>
-      </c>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
       <c r="Y13" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z13" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA13" s="3"/>
-    </row>
-    <row r="14" spans="1:27" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="12"/>
+    </row>
+    <row r="14" spans="1:27" s="11" customFormat="1" ht="27" customHeight="1">
       <c r="A14" s="8"/>
-      <c r="B14" s="4" t="s">
-        <v>136</v>
+      <c r="B14" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="C14" s="8">
-        <v>79566</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>109</v>
-      </c>
+        <v>70271</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="8"/>
       <c r="F14" s="8" t="s">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J14" s="8">
-        <v>32</v>
+      <c r="J14" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
-      <c r="N14" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="O14" s="8"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="8" t="s">
+        <v>77</v>
+      </c>
       <c r="P14" s="8"/>
-      <c r="Q14" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="R14" s="8" t="s">
-        <v>113</v>
-      </c>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
       <c r="S14" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="T14" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="U14" s="8" t="s">
-        <v>116</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
       <c r="V14" s="8"/>
       <c r="W14" s="8"/>
       <c r="X14" s="8"/>
-      <c r="Y14" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="Y14" s="8"/>
       <c r="Z14" s="8"/>
       <c r="AA14" s="12"/>
     </row>
-    <row r="15" spans="1:27" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="27" customHeight="1">
       <c r="A15" s="8"/>
-      <c r="B15" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C15" s="8">
-        <v>79566</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>109</v>
-      </c>
+      <c r="B15" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="8"/>
       <c r="F15" s="8" t="s">
-        <v>110</v>
+        <v>28</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J15" s="8">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="R15" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="S15" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="T15" s="8" t="s">
-        <v>115</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
       <c r="U15" s="8" t="s">
-        <v>116</v>
+        <v>48</v>
       </c>
       <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="8"/>
+      <c r="W15" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X15" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="Y15" s="8" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="Z15" s="8"/>
-      <c r="AA15" s="12"/>
-    </row>
-    <row r="16" spans="1:27" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA15" s="3"/>
+    </row>
+    <row r="16" spans="1:27" ht="27" customHeight="1">
       <c r="A16" s="8"/>
-      <c r="B16" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C16" s="8">
-        <v>70271</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>73</v>
+      <c r="B16" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="I16" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="I16" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J16" s="8" t="s">
-        <v>75</v>
+      <c r="J16" s="8">
+        <v>28</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
+        <v>39</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="N16" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="O16" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
+        <v>119</v>
+      </c>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="V16" s="8"/>
-      <c r="W16" s="8"/>
-      <c r="X16" s="8"/>
-      <c r="Y16" s="8"/>
+      <c r="W16" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X16" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y16" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="Z16" s="8"/>
-      <c r="AA16" s="12"/>
-    </row>
-    <row r="17" spans="1:27" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA16" s="3"/>
+    </row>
+    <row r="17" spans="1:27" ht="27" customHeight="1">
       <c r="A17" s="8"/>
-      <c r="B17" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C17" s="8">
-        <v>70271</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>73</v>
+      <c r="B17" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="I17" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J17" s="8" t="s">
-        <v>75</v>
+      <c r="J17" s="8">
+        <v>28</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
+        <v>39</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="V17" s="8"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="8"/>
-      <c r="Y17" s="8"/>
+      <c r="W17" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X17" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y17" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="Z17" s="8"/>
-      <c r="AA17" s="12"/>
-    </row>
-    <row r="18" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA17" s="3"/>
+    </row>
+    <row r="18" spans="1:27" ht="27" customHeight="1">
       <c r="A18" s="8"/>
       <c r="B18" s="14" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8" t="s">
@@ -1944,7 +1902,7 @@
         <v>29</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>38</v>
@@ -1986,10 +1944,10 @@
       <c r="Z18" s="8"/>
       <c r="AA18" s="3"/>
     </row>
-    <row r="19" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" ht="27" customHeight="1">
       <c r="A19" s="8"/>
       <c r="B19" s="14" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8" t="s">
@@ -2000,10 +1958,10 @@
         <v>28</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>29</v>
+        <v>127</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="I19" s="8" t="s">
         <v>38</v>
@@ -2045,10 +2003,10 @@
       <c r="Z19" s="8"/>
       <c r="AA19" s="3"/>
     </row>
-    <row r="20" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" ht="27" customHeight="1">
       <c r="A20" s="8"/>
       <c r="B20" s="14" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8" t="s">
@@ -2059,10 +2017,10 @@
         <v>28</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>29</v>
+        <v>127</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>38</v>
@@ -2104,10 +2062,10 @@
       <c r="Z20" s="8"/>
       <c r="AA20" s="3"/>
     </row>
-    <row r="21" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" ht="27" customHeight="1">
       <c r="A21" s="8"/>
       <c r="B21" s="14" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8" t="s">
@@ -2121,13 +2079,13 @@
         <v>29</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J21" s="8">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>39</v>
@@ -2163,10 +2121,10 @@
       <c r="Z21" s="8"/>
       <c r="AA21" s="3"/>
     </row>
-    <row r="22" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" ht="27" customHeight="1">
       <c r="A22" s="8"/>
       <c r="B22" s="14" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8" t="s">
@@ -2177,16 +2135,16 @@
         <v>28</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>127</v>
+        <v>29</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J22" s="8">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="K22" s="8" t="s">
         <v>39</v>
@@ -2198,7 +2156,7 @@
         <v>47</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
@@ -2222,10 +2180,10 @@
       <c r="Z22" s="8"/>
       <c r="AA22" s="3"/>
     </row>
-    <row r="23" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" ht="27" customHeight="1">
       <c r="A23" s="8"/>
       <c r="B23" s="14" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8" t="s">
@@ -2236,16 +2194,16 @@
         <v>28</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>127</v>
+        <v>29</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J23" s="8">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>39</v>
@@ -2257,7 +2215,7 @@
         <v>47</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
@@ -2281,183 +2239,6 @@
       <c r="Z23" s="8"/>
       <c r="AA23" s="3"/>
     </row>
-    <row r="24" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="I24" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="J24" s="8">
-        <v>32</v>
-      </c>
-      <c r="K24" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="L24" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="M24" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="N24" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
-      <c r="U24" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="V24" s="8"/>
-      <c r="W24" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="X24" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y24" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z24" s="8"/>
-      <c r="AA24" s="3"/>
-    </row>
-    <row r="25" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="J25" s="8">
-        <v>32</v>
-      </c>
-      <c r="K25" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="L25" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="M25" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="N25" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
-      <c r="U25" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="V25" s="8"/>
-      <c r="W25" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="X25" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y25" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z25" s="8"/>
-      <c r="AA25" s="3"/>
-    </row>
-    <row r="26" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H26" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="I26" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="J26" s="8">
-        <v>32</v>
-      </c>
-      <c r="K26" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="L26" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="M26" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="N26" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
-      <c r="U26" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="V26" s="8"/>
-      <c r="W26" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="X26" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y26" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z26" s="8"/>
-      <c r="AA26" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
gse english new file added
</commit_message>
<xml_diff>
--- a/src/main/java/lomt/pearson/fileupload/english/gse/ingestion/Gse_Ingestion_Template.xlsx
+++ b/src/main/java/lomt/pearson/fileupload/english/gse/ingestion/Gse_Ingestion_Template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="166">
   <si>
     <t>To be populated - ignored by the import</t>
   </si>
@@ -259,9 +259,6 @@
     <t>ad | advertise | agency | brochure | leaflet</t>
   </si>
   <si>
-    <t>GLSI6666B0</t>
-  </si>
-  <si>
     <t>GLSI2222C0</t>
   </si>
   <si>
@@ -301,9 +298,6 @@
     <t>Academic Text Strategies&gt;Skimming for main idea/gist|Academic strategies&gt;Summarising|Academic Text Strategies&gt;Prediction</t>
   </si>
   <si>
-    <t>GLSI6666A0</t>
-  </si>
-  <si>
     <t>Can respond to ideas and suggestions in informal discussions UPDATE 24</t>
   </si>
   <si>
@@ -343,9 +337,6 @@
     <t>Source Descriptor updated</t>
   </si>
   <si>
-    <t>GLGR0027</t>
-  </si>
-  <si>
     <t>GLGR</t>
   </si>
   <si>
@@ -424,6 +415,24 @@
     <t>GLSI16099C0</t>
   </si>
   <si>
+    <t>GLSI16098C0</t>
+  </si>
+  <si>
+    <t>GLSI6666D0</t>
+  </si>
+  <si>
+    <t>GLSI6666Q0</t>
+  </si>
+  <si>
+    <t>GLGR0029</t>
+  </si>
+  <si>
+    <t>(E)</t>
+  </si>
+  <si>
+    <t>(EA)</t>
+  </si>
+  <si>
     <t>GLSI0219c|98765</t>
   </si>
   <si>
@@ -487,58 +496,28 @@
     <t>Can use language related to adverts and brands 29 Jan</t>
   </si>
   <si>
-    <t>(C)</t>
-  </si>
-  <si>
     <t>43-58</t>
   </si>
   <si>
-    <t>GLSI3181f1</t>
-  </si>
-  <si>
-    <t>GLSI3181f2</t>
-  </si>
-  <si>
-    <t>YLLA01f3</t>
-  </si>
-  <si>
-    <t>GLGR051f4</t>
-  </si>
-  <si>
-    <t>GLGR051f5</t>
-  </si>
-  <si>
-    <t>GLVC561f6</t>
-  </si>
-  <si>
-    <t>GLVC561f7</t>
-  </si>
-  <si>
-    <t>GLSI3181g1</t>
-  </si>
-  <si>
-    <t>GLSI3181g2</t>
-  </si>
-  <si>
-    <t>YLLA01g3</t>
-  </si>
-  <si>
-    <t>GLGR051g4</t>
-  </si>
-  <si>
-    <t>GLGR051g5</t>
-  </si>
-  <si>
-    <t>GLVC561g6</t>
-  </si>
-  <si>
-    <t>GLVC561g7</t>
-  </si>
-  <si>
-    <t>(E)</t>
-  </si>
-  <si>
-    <t>(EA)</t>
+    <t>GLSI3181k1</t>
+  </si>
+  <si>
+    <t>GLSI3181k2</t>
+  </si>
+  <si>
+    <t>YLLA01k3</t>
+  </si>
+  <si>
+    <t>GLGR051k4</t>
+  </si>
+  <si>
+    <t>GLGR051k5</t>
+  </si>
+  <si>
+    <t>GLVC561k6</t>
+  </si>
+  <si>
+    <t>GLVC561k7</t>
   </si>
 </sst>
 </file>
@@ -615,14 +594,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD0E0E3"/>
-        <bgColor rgb="FFD0E0E3"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFD0E0E3"/>
+        <bgColor rgb="FFD0E0E3"/>
       </patternFill>
     </fill>
   </fills>
@@ -656,7 +635,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -700,14 +679,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -771,7 +753,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -806,7 +788,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1015,10 +997,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA37"/>
+  <dimension ref="A1:AA31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1089,7 +1071,7 @@
         <v>13</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>14</v>
@@ -1132,17 +1114,15 @@
     <row r="2" spans="1:27" ht="27" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="14" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>134</v>
+        <v>26</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>135</v>
-      </c>
+      <c r="E2" s="8"/>
       <c r="F2" s="8" t="s">
         <v>28</v>
       </c>
@@ -1150,25 +1130,25 @@
         <v>29</v>
       </c>
       <c r="H2" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>136</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="J2" s="8">
         <v>55</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>137</v>
+        <v>31</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>138</v>
+        <v>101</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>139</v>
+        <v>32</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
@@ -1177,20 +1157,14 @@
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
       <c r="U2" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="V2" s="8" t="s">
-        <v>140</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="V2" s="8"/>
       <c r="W2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="Y2" s="8" t="s">
-        <v>56</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
       <c r="Z2" s="8" t="s">
         <v>34</v>
       </c>
@@ -1199,13 +1173,17 @@
     <row r="3" spans="1:27" ht="27" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="C3" s="8"/>
+        <v>133</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="F3" s="8" t="s">
         <v>28</v>
       </c>
@@ -1213,12 +1191,18 @@
         <v>29</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="10"/>
+        <v>93</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="J3" s="8">
+        <v>27</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="9"/>
       <c r="O3" s="4"/>
@@ -1229,368 +1213,399 @@
       <c r="T3" s="4"/>
       <c r="U3" s="8"/>
       <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
+      <c r="W3" s="8" t="s">
+        <v>104</v>
+      </c>
       <c r="X3" s="8"/>
       <c r="Y3" s="8"/>
       <c r="Z3" s="8"/>
       <c r="AA3" s="3"/>
     </row>
-    <row r="4" spans="1:27" customFormat="1" ht="27" customHeight="1">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G4" s="4" t="s">
+    <row r="4" spans="1:27" ht="27" customHeight="1">
+      <c r="A4" s="8"/>
+      <c r="B4" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="J4" s="4">
+      <c r="H4" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="8">
+        <v>60</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
+      <c r="M4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="X4" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="Y4" s="15"/>
-      <c r="Z4" s="3"/>
-    </row>
-    <row r="5" spans="1:27" s="11" customFormat="1" ht="27" customHeight="1">
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="X4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="3"/>
+    </row>
+    <row r="5" spans="1:27" ht="27" customHeight="1">
       <c r="A5" s="8"/>
-      <c r="B5" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="B5" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="8"/>
       <c r="D5" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>150</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E5" s="8"/>
       <c r="F5" s="8" t="s">
-        <v>110</v>
+        <v>28</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>151</v>
+        <v>95</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J5" s="8">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
+        <v>39</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="N5" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="R5" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="S5" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="T5" s="8" t="s">
-        <v>115</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
       <c r="U5" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="V5" s="8" t="s">
-        <v>140</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="V5" s="8"/>
       <c r="W5" s="8" t="s">
-        <v>141</v>
+        <v>49</v>
       </c>
       <c r="X5" s="8" t="s">
-        <v>142</v>
+        <v>50</v>
       </c>
       <c r="Y5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA5" s="12"/>
-    </row>
-    <row r="6" spans="1:27" s="11" customFormat="1" ht="27" customHeight="1">
+        <v>39</v>
+      </c>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="3"/>
+    </row>
+    <row r="6" spans="1:27" ht="27" customHeight="1">
       <c r="A6" s="8"/>
-      <c r="B6" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="C6" s="8"/>
+      <c r="B6" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="D6" s="8" t="s">
-        <v>108</v>
+        <v>27</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>150</v>
+        <v>42</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>110</v>
+        <v>28</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
+        <v>96</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="8">
+        <v>69</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
       <c r="U6" s="8"/>
       <c r="V6" s="8"/>
-      <c r="W6" s="8"/>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="8"/>
+      <c r="W6" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="X6" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y6" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="Z6" s="8"/>
-      <c r="AA6" s="12"/>
-    </row>
-    <row r="7" spans="1:27" s="11" customFormat="1" ht="27" customHeight="1">
+      <c r="AA6" s="3"/>
+    </row>
+    <row r="7" spans="1:27" ht="27" customHeight="1">
       <c r="A7" s="8"/>
-      <c r="B7" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>153</v>
-      </c>
+      <c r="B7" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="8"/>
       <c r="D7" s="8" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>127</v>
+        <v>29</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>154</v>
+        <v>97</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>156</v>
+        <v>38</v>
+      </c>
+      <c r="J7" s="8">
+        <v>32</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="O7" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8" t="s">
-        <v>140</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="V7" s="8"/>
       <c r="W7" s="8"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="8"/>
-      <c r="Z7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA7" s="12"/>
-    </row>
-    <row r="8" spans="1:27" s="11" customFormat="1" ht="27" customHeight="1">
+      <c r="X7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="3"/>
+    </row>
+    <row r="8" spans="1:27" ht="27" customHeight="1">
       <c r="A8" s="8"/>
-      <c r="B8" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="C8" s="8"/>
+      <c r="B8" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="D8" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" s="8"/>
+        <v>27</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="F8" s="8" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>127</v>
+        <v>29</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
+        <v>98</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="8">
+        <v>72</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
       <c r="U8" s="8"/>
       <c r="V8" s="8"/>
       <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
+      <c r="X8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y8" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="Z8" s="8"/>
-      <c r="AA8" s="12"/>
+      <c r="AA8" s="3"/>
     </row>
     <row r="9" spans="1:27" ht="27" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>26</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="C9" s="8"/>
       <c r="D9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="8"/>
+      <c r="E9" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="F9" s="8" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="J9" s="8">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="L9" s="10" t="s">
-        <v>103</v>
+        <v>39</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="N9" s="9" t="s">
-        <v>104</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
-      <c r="U9" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="U9" s="8"/>
       <c r="V9" s="8"/>
       <c r="W9" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="8"/>
-      <c r="Z9" s="8" t="s">
-        <v>34</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="X9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z9" s="8"/>
       <c r="AA9" s="3"/>
     </row>
     <row r="10" spans="1:27" ht="27" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>35</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C10" s="8"/>
       <c r="D10" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J10" s="8">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K10" s="8" t="s">
         <v>39</v>
       </c>
       <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="9"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
@@ -1600,17 +1615,23 @@
       <c r="U10" s="8"/>
       <c r="V10" s="8"/>
       <c r="W10" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="X10" s="8"/>
-      <c r="Y10" s="8"/>
-      <c r="Z10" s="8"/>
+        <v>68</v>
+      </c>
+      <c r="X10" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z10" s="8" t="s">
+        <v>69</v>
+      </c>
       <c r="AA10" s="3"/>
     </row>
     <row r="11" spans="1:27" ht="27" customHeight="1">
       <c r="A11" s="8"/>
       <c r="B11" s="14" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8" t="s">
@@ -1623,29 +1644,23 @@
         <v>28</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J11" s="8">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>90</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="L11" s="8"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
@@ -1655,208 +1670,196 @@
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
       <c r="W11" s="8" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="X11" s="8" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="Y11" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z11" s="8"/>
+        <v>58</v>
+      </c>
+      <c r="Z11" s="8" t="s">
+        <v>72</v>
+      </c>
       <c r="AA11" s="3"/>
     </row>
     <row r="12" spans="1:27" ht="27" customHeight="1">
       <c r="A12" s="8"/>
       <c r="B12" s="14" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="F12" s="8" t="s">
         <v>28</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J12" s="8">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="N12" s="5" t="s">
-        <v>119</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="L12" s="8"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
-      <c r="U12" s="8" t="s">
-        <v>48</v>
-      </c>
+      <c r="U12" s="8"/>
       <c r="V12" s="8"/>
       <c r="W12" s="8" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="X12" s="8" t="s">
         <v>50</v>
       </c>
       <c r="Y12" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z12" s="8"/>
+        <v>58</v>
+      </c>
+      <c r="Z12" s="8" t="s">
+        <v>72</v>
+      </c>
       <c r="AA12" s="3"/>
     </row>
-    <row r="13" spans="1:27" ht="27" customHeight="1">
+    <row r="13" spans="1:27" s="11" customFormat="1" ht="27" customHeight="1">
       <c r="A13" s="8"/>
-      <c r="B13" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>51</v>
+      <c r="B13" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13" s="8">
+        <v>79566</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>27</v>
+        <v>105</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>28</v>
+        <v>107</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>38</v>
+        <v>135</v>
       </c>
       <c r="J13" s="8">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="N13" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="8"/>
+        <v>56</v>
+      </c>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="R13" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="S13" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="T13" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="U13" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="V13" s="8"/>
-      <c r="W13" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="X13" s="8" t="s">
-        <v>55</v>
-      </c>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
       <c r="Y13" s="8" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="Z13" s="8"/>
-      <c r="AA13" s="3"/>
-    </row>
-    <row r="14" spans="1:27" ht="27" customHeight="1">
+      <c r="AA13" s="12"/>
+    </row>
+    <row r="14" spans="1:27" s="11" customFormat="1" ht="27" customHeight="1">
       <c r="A14" s="8"/>
-      <c r="B14" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C14" s="8"/>
+      <c r="B14" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" s="8">
+        <v>70271</v>
+      </c>
       <c r="D14" s="8" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J14" s="8">
-        <v>32</v>
+      <c r="J14" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="L14" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="M14" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="N14" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="8" t="s">
-        <v>61</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
       <c r="V14" s="8"/>
       <c r="W14" s="8"/>
-      <c r="X14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y14" s="8" t="s">
-        <v>39</v>
-      </c>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
       <c r="Z14" s="8"/>
-      <c r="AA14" s="3"/>
+      <c r="AA14" s="12"/>
     </row>
     <row r="15" spans="1:27" ht="27" customHeight="1">
       <c r="A15" s="8"/>
       <c r="B15" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>62</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="C15" s="8"/>
       <c r="D15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="E15" s="8"/>
       <c r="F15" s="8" t="s">
         <v>28</v>
       </c>
@@ -1864,25 +1867,25 @@
         <v>29</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J15" s="8">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="N15" s="8" t="s">
-        <v>92</v>
+        <v>47</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>116</v>
       </c>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
@@ -1890,14 +1893,18 @@
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
       <c r="T15" s="4"/>
-      <c r="U15" s="8"/>
+      <c r="U15" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
+      <c r="W15" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="X15" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="Y15" s="8" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="Z15" s="8"/>
       <c r="AA15" s="3"/>
@@ -1905,50 +1912,52 @@
     <row r="16" spans="1:27" ht="27" customHeight="1">
       <c r="A16" s="8"/>
       <c r="B16" s="14" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="E16" s="8"/>
       <c r="F16" s="8" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J16" s="8">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>39</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="N16" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
       <c r="T16" s="4"/>
-      <c r="U16" s="8"/>
+      <c r="U16" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="V16" s="8"/>
       <c r="W16" s="8" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="X16" s="8" t="s">
         <v>50</v>
@@ -1962,46 +1971,52 @@
     <row r="17" spans="1:27" ht="27" customHeight="1">
       <c r="A17" s="8"/>
       <c r="B17" s="14" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="E17" s="8"/>
       <c r="F17" s="8" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="I17" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J17" s="8">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K17" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="L17" s="8"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
+      <c r="L17" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
-      <c r="U17" s="8"/>
+      <c r="U17" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="V17" s="8"/>
       <c r="W17" s="8" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="X17" s="8" t="s">
         <v>50</v>
@@ -2009,237 +2024,249 @@
       <c r="Y17" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="Z17" s="8" t="s">
-        <v>69</v>
-      </c>
+      <c r="Z17" s="8"/>
       <c r="AA17" s="3"/>
     </row>
     <row r="18" spans="1:27" ht="27" customHeight="1">
       <c r="A18" s="8"/>
       <c r="B18" s="14" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="E18" s="8"/>
       <c r="F18" s="8" t="s">
         <v>28</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J18" s="8">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="L18" s="8"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M18" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
-      <c r="U18" s="8"/>
+      <c r="U18" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="V18" s="8"/>
       <c r="W18" s="8" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="X18" s="8" t="s">
         <v>50</v>
       </c>
       <c r="Y18" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z18" s="8" t="s">
-        <v>72</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="Z18" s="8"/>
       <c r="AA18" s="3"/>
     </row>
     <row r="19" spans="1:27" ht="27" customHeight="1">
       <c r="A19" s="8"/>
       <c r="B19" s="14" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="E19" s="8"/>
       <c r="F19" s="8" t="s">
         <v>28</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="I19" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J19" s="8">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="L19" s="8"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
       <c r="T19" s="4"/>
-      <c r="U19" s="8"/>
+      <c r="U19" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="V19" s="8"/>
       <c r="W19" s="8" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="X19" s="8" t="s">
         <v>50</v>
       </c>
       <c r="Y19" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z19" s="8" t="s">
-        <v>72</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="Z19" s="8"/>
       <c r="AA19" s="3"/>
     </row>
-    <row r="20" spans="1:27" s="11" customFormat="1" ht="27" customHeight="1">
+    <row r="20" spans="1:27" ht="27" customHeight="1">
       <c r="A20" s="8"/>
-      <c r="B20" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" s="8">
-        <v>79566</v>
-      </c>
+      <c r="B20" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" s="8"/>
       <c r="D20" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>109</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E20" s="8"/>
       <c r="F20" s="8" t="s">
-        <v>110</v>
+        <v>28</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J20" s="8">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="R20" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="S20" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="T20" s="8" t="s">
-        <v>115</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
       <c r="U20" s="8" t="s">
-        <v>116</v>
+        <v>48</v>
       </c>
       <c r="V20" s="8"/>
-      <c r="W20" s="8"/>
-      <c r="X20" s="8"/>
+      <c r="W20" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X20" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="Y20" s="8" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="Z20" s="8"/>
-      <c r="AA20" s="12"/>
-    </row>
-    <row r="21" spans="1:27" s="11" customFormat="1" ht="27" customHeight="1">
+      <c r="AA20" s="3"/>
+    </row>
+    <row r="21" spans="1:27" ht="27" customHeight="1">
       <c r="A21" s="8"/>
-      <c r="B21" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" s="8">
-        <v>70271</v>
-      </c>
+      <c r="B21" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="8"/>
       <c r="D21" s="8" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J21" s="8" t="s">
-        <v>75</v>
+      <c r="J21" s="8">
+        <v>32</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="T21" s="8"/>
-      <c r="U21" s="8"/>
+        <v>39</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M21" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N21" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="V21" s="8"/>
-      <c r="W21" s="8"/>
-      <c r="X21" s="8"/>
-      <c r="Y21" s="8"/>
+      <c r="W21" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X21" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y21" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="Z21" s="8"/>
-      <c r="AA21" s="12"/>
+      <c r="AA21" s="3"/>
     </row>
     <row r="22" spans="1:27" ht="27" customHeight="1">
       <c r="A22" s="8"/>
       <c r="B22" s="14" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8" t="s">
@@ -2253,13 +2280,13 @@
         <v>29</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J22" s="8">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="K22" s="8" t="s">
         <v>39</v>
@@ -2271,7 +2298,7 @@
         <v>47</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
@@ -2298,7 +2325,7 @@
     <row r="23" spans="1:27" ht="27" customHeight="1">
       <c r="A23" s="8"/>
       <c r="B23" s="14" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8" t="s">
@@ -2312,13 +2339,13 @@
         <v>29</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J23" s="8">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>39</v>
@@ -2330,7 +2357,7 @@
         <v>47</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
@@ -2357,7 +2384,7 @@
     <row r="24" spans="1:27" ht="27" customHeight="1">
       <c r="A24" s="8"/>
       <c r="B24" s="14" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8" t="s">
@@ -2371,13 +2398,13 @@
         <v>29</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J24" s="8">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="K24" s="8" t="s">
         <v>39</v>
@@ -2389,7 +2416,7 @@
         <v>47</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
@@ -2415,14 +2442,18 @@
     </row>
     <row r="25" spans="1:27" ht="27" customHeight="1">
       <c r="A25" s="8"/>
-      <c r="B25" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="C25" s="8"/>
+      <c r="B25" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>137</v>
+      </c>
       <c r="D25" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="8"/>
+      <c r="E25" s="8" t="s">
+        <v>138</v>
+      </c>
       <c r="F25" s="8" t="s">
         <v>28</v>
       </c>
@@ -2430,25 +2461,25 @@
         <v>29</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="J25" s="8">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="L25" s="8" t="s">
-        <v>46</v>
+        <v>140</v>
+      </c>
+      <c r="L25" s="10" t="s">
+        <v>141</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="N25" s="5" t="s">
-        <v>119</v>
+        <v>142</v>
+      </c>
+      <c r="N25" s="9" t="s">
+        <v>102</v>
       </c>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
@@ -2457,25 +2488,29 @@
       <c r="S25" s="4"/>
       <c r="T25" s="4"/>
       <c r="U25" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="V25" s="8"/>
+        <v>113</v>
+      </c>
+      <c r="V25" s="8" t="s">
+        <v>143</v>
+      </c>
       <c r="W25" s="8" t="s">
-        <v>49</v>
+        <v>144</v>
       </c>
       <c r="X25" s="8" t="s">
-        <v>50</v>
+        <v>145</v>
       </c>
       <c r="Y25" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z25" s="8"/>
+        <v>56</v>
+      </c>
+      <c r="Z25" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="AA25" s="3"/>
     </row>
     <row r="26" spans="1:27" ht="27" customHeight="1">
       <c r="A26" s="8"/>
       <c r="B26" s="14" t="s">
-        <v>126</v>
+        <v>160</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8" t="s">
@@ -2486,654 +2521,292 @@
         <v>28</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>127</v>
+        <v>29</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="I26" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="J26" s="8">
-        <v>28</v>
-      </c>
-      <c r="K26" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="L26" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="M26" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="N26" s="5" t="s">
-        <v>119</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="9"/>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
       <c r="S26" s="4"/>
       <c r="T26" s="4"/>
-      <c r="U26" s="8" t="s">
-        <v>48</v>
-      </c>
+      <c r="U26" s="8"/>
       <c r="V26" s="8"/>
-      <c r="W26" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="X26" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y26" s="8" t="s">
-        <v>39</v>
-      </c>
+      <c r="W26" s="8"/>
+      <c r="X26" s="8"/>
+      <c r="Y26" s="8"/>
       <c r="Z26" s="8"/>
       <c r="AA26" s="3"/>
     </row>
-    <row r="27" spans="1:27" ht="27" customHeight="1">
-      <c r="A27" s="8"/>
-      <c r="B27" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="I27" s="8" t="s">
+    <row r="27" spans="1:27" customFormat="1" ht="27" customHeight="1">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="I27" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="J27" s="8">
-        <v>28</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="L27" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="M27" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="N27" s="5" t="s">
-        <v>119</v>
-      </c>
+      <c r="J27" s="4">
+        <v>44</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
       <c r="S27" s="4"/>
       <c r="T27" s="4"/>
-      <c r="U27" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="V27" s="8"/>
-      <c r="W27" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="X27" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y27" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z27" s="8"/>
-      <c r="AA27" s="3"/>
-    </row>
-    <row r="28" spans="1:27" ht="27" customHeight="1">
+      <c r="U27" s="4"/>
+      <c r="V27" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="W27" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="X27" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y27" s="16"/>
+      <c r="Z27" s="3"/>
+    </row>
+    <row r="28" spans="1:27" s="11" customFormat="1" ht="27" customHeight="1">
       <c r="A28" s="8"/>
-      <c r="B28" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="C28" s="8"/>
+      <c r="B28" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>152</v>
+      </c>
       <c r="D28" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E28" s="8"/>
+        <v>105</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>153</v>
+      </c>
       <c r="F28" s="8" t="s">
-        <v>28</v>
+        <v>107</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>38</v>
+        <v>136</v>
       </c>
       <c r="J28" s="8">
         <v>32</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="L28" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="M28" s="8" t="s">
-        <v>47</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
       <c r="N28" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
+        <v>116</v>
+      </c>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="R28" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="S28" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="T28" s="8" t="s">
+        <v>112</v>
+      </c>
       <c r="U28" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="V28" s="8"/>
+        <v>113</v>
+      </c>
+      <c r="V28" s="8" t="s">
+        <v>143</v>
+      </c>
       <c r="W28" s="8" t="s">
-        <v>49</v>
+        <v>144</v>
       </c>
       <c r="X28" s="8" t="s">
-        <v>50</v>
+        <v>145</v>
       </c>
       <c r="Y28" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z28" s="8"/>
-      <c r="AA28" s="3"/>
-    </row>
-    <row r="29" spans="1:27" ht="27" customHeight="1">
+        <v>56</v>
+      </c>
+      <c r="Z28" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA28" s="12"/>
+    </row>
+    <row r="29" spans="1:27" s="11" customFormat="1" ht="27" customHeight="1">
       <c r="A29" s="8"/>
-      <c r="B29" s="14" t="s">
-        <v>131</v>
+      <c r="B29" s="8" t="s">
+        <v>163</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E29" s="8"/>
+        <v>105</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>153</v>
+      </c>
       <c r="F29" s="8" t="s">
-        <v>28</v>
+        <v>107</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="J29" s="8">
-        <v>32</v>
-      </c>
-      <c r="K29" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="L29" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="M29" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="N29" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="U29" s="8" t="s">
-        <v>48</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="17"/>
+      <c r="S29" s="8"/>
+      <c r="T29" s="8"/>
+      <c r="U29" s="8"/>
       <c r="V29" s="8"/>
-      <c r="W29" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="X29" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y29" s="8" t="s">
-        <v>39</v>
-      </c>
+      <c r="W29" s="8"/>
+      <c r="X29" s="8"/>
+      <c r="Y29" s="8"/>
       <c r="Z29" s="8"/>
-      <c r="AA29" s="3"/>
-    </row>
-    <row r="30" spans="1:27" ht="27" customHeight="1">
+      <c r="AA29" s="12"/>
+    </row>
+    <row r="30" spans="1:27" s="11" customFormat="1" ht="27" customHeight="1">
       <c r="A30" s="8"/>
-      <c r="B30" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="C30" s="8"/>
+      <c r="B30" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>156</v>
+      </c>
       <c r="D30" s="8" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="8" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="J30" s="8">
-        <v>32</v>
+        <v>135</v>
+      </c>
+      <c r="J30" s="18" t="s">
+        <v>158</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="L30" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="M30" s="8" t="s">
-        <v>47</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
       <c r="N30" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="4"/>
-      <c r="S30" s="4"/>
-      <c r="T30" s="4"/>
-      <c r="U30" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="V30" s="8"/>
-      <c r="W30" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="X30" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y30" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z30" s="8"/>
-      <c r="AA30" s="3"/>
-    </row>
-    <row r="31" spans="1:27" ht="27" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="O30" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="T30" s="8"/>
+      <c r="U30" s="8"/>
+      <c r="V30" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="W30" s="8"/>
+      <c r="X30" s="8"/>
+      <c r="Y30" s="8"/>
+      <c r="Z30" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA30" s="12"/>
+    </row>
+    <row r="31" spans="1:27" s="11" customFormat="1" ht="27" customHeight="1">
       <c r="A31" s="8"/>
-      <c r="B31" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>134</v>
-      </c>
+      <c r="B31" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C31" s="8"/>
       <c r="D31" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>135</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="E31" s="8"/>
       <c r="F31" s="8" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J31" s="8">
-        <v>55</v>
-      </c>
-      <c r="K31" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="L31" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="M31" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="N31" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
-      <c r="U31" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="V31" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="W31" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="X31" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="Y31" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z31" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA31" s="3"/>
-    </row>
-    <row r="32" spans="1:27" ht="27" customHeight="1">
-      <c r="A32" s="8"/>
-      <c r="B32" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H32" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
-      <c r="U32" s="8"/>
-      <c r="V32" s="8"/>
-      <c r="W32" s="8"/>
-      <c r="X32" s="8"/>
-      <c r="Y32" s="8"/>
-      <c r="Z32" s="8"/>
-      <c r="AA32" s="3"/>
-    </row>
-    <row r="33" spans="1:27" customFormat="1" ht="27" customHeight="1">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H33" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J33" s="4">
-        <v>44</v>
-      </c>
-      <c r="K33" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="T33" s="4"/>
-      <c r="U33" s="4"/>
-      <c r="V33" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="W33" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="X33" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="Y33" s="15"/>
-      <c r="Z33" s="3"/>
-    </row>
-    <row r="34" spans="1:27" s="11" customFormat="1" ht="27" customHeight="1">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H34" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="J34" s="8">
-        <v>32</v>
-      </c>
-      <c r="K34" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="R34" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="S34" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="T34" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="U34" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="V34" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="W34" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="X34" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="Y34" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z34" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA34" s="12"/>
-    </row>
-    <row r="35" spans="1:27" s="11" customFormat="1" ht="27" customHeight="1">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H35" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="5"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="16"/>
-      <c r="S35" s="8"/>
-      <c r="T35" s="8"/>
-      <c r="U35" s="8"/>
-      <c r="V35" s="8"/>
-      <c r="W35" s="8"/>
-      <c r="X35" s="8"/>
-      <c r="Y35" s="8"/>
-      <c r="Z35" s="8"/>
-      <c r="AA35" s="12"/>
-    </row>
-    <row r="36" spans="1:27" s="11" customFormat="1" ht="27" customHeight="1">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="H36" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="I36" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="J36" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="K36" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="O36" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="T36" s="8"/>
-      <c r="U36" s="8"/>
-      <c r="V36" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="W36" s="8"/>
-      <c r="X36" s="8"/>
-      <c r="Y36" s="8"/>
-      <c r="Z36" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA36" s="12"/>
-    </row>
-    <row r="37" spans="1:27" s="11" customFormat="1" ht="27" customHeight="1">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="H37" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="I37" s="8"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="8"/>
-      <c r="S37" s="8"/>
-      <c r="T37" s="8"/>
-      <c r="U37" s="8"/>
-      <c r="V37" s="8"/>
-      <c r="W37" s="8"/>
-      <c r="X37" s="8"/>
-      <c r="Y37" s="8"/>
-      <c r="Z37" s="8"/>
-      <c r="AA37" s="12"/>
+        <v>157</v>
+      </c>
+      <c r="I31" s="8"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="8"/>
+      <c r="S31" s="8"/>
+      <c r="T31" s="8"/>
+      <c r="U31" s="8"/>
+      <c r="V31" s="8"/>
+      <c r="W31" s="8"/>
+      <c r="X31" s="8"/>
+      <c r="Y31" s="8"/>
+      <c r="Z31" s="8"/>
+      <c r="AA31" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>